<commit_message>
user delete some text
</commit_message>
<xml_diff>
--- a/New data.xlsx
+++ b/New data.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="179" uniqueCount="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="178" uniqueCount="105">
   <si>
     <t>Time</t>
   </si>
@@ -331,9 +331,6 @@
   </si>
   <si>
     <t>Umar ali</t>
-  </si>
-  <si>
-    <t>her we collect new data</t>
   </si>
 </sst>
 </file>
@@ -3226,9 +3223,7 @@
       <c r="C27" s="11">
         <v>73112</v>
       </c>
-      <c r="D27" s="24" t="s">
-        <v>105</v>
-      </c>
+      <c r="D27" s="24"/>
     </row>
     <row r="28" spans="1:4" ht="18.5">
       <c r="A28" s="4">

</xml_diff>